<commit_message>
ATA do dia 18/10 e link dos slides de apresentacao
</commit_message>
<xml_diff>
--- a/Documentação/ATAs_de_Reuniao/Sprint 2/Semana 1010/Grupo4_ATA_Semana1010.xlsx
+++ b/Documentação/ATAs_de_Reuniao/Sprint 2/Semana 1010/Grupo4_ATA_Semana1010.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSCode\SPTECH\GitHub\Sprint-2\ATAs_de_Reuniao\Sprint 2\Semana 1010\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpfer\OneDrive\Documentos\SPTECH\PI\SPRINT\Sprint-SPTECH\Documentação\ATAs_de_Reuniao\Sprint 2\Semana 1010\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7996218A-87FD-4A81-88D4-59BAD373E7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3E68C8-49F1-4090-BEAF-5EAAC91AB15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="4824" yWindow="3360" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="2" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DE DADOS" sheetId="2" state="hidden" r:id="rId1"/>
     <sheet name="Quinta" sheetId="1" r:id="rId2"/>
-    <sheet name="Sexta" sheetId="11" r:id="rId3"/>
+    <sheet name="Sexta" sheetId="19" r:id="rId3"/>
     <sheet name="Sábado" sheetId="17" r:id="rId4"/>
     <sheet name="Segunda" sheetId="13" r:id="rId5"/>
     <sheet name="Terça" sheetId="18" r:id="rId6"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="68">
   <si>
     <t>NOME</t>
   </si>
@@ -234,9 +234,6 @@
     <t>16/10/2024</t>
   </si>
   <si>
-    <t>Mediante a semana de home office, foi acertado os horários para reuniões diárias serão por volta das 11h, junto da tarefa de criar o slide de apresentação e foi marcado o primeiro ensaio para a apresentação do da Sprint, na sexta feira dia 18/10.</t>
-  </si>
-  <si>
     <t>Conferimos novamente o que estava pendente no trabalho. Cada membro comunicou o que seria feito durante o fim de semana para apresentarmos na próxima daily, na segunda-feira.</t>
   </si>
   <si>
@@ -244,6 +241,12 @@
   </si>
   <si>
     <t>Foi falado sobre a possível ordem de apresentação dos slides no dia da sprint, revisitamos algumas areas do site, apontando mudanças que deveram ser feitas. Ao final, foi decidido que todas as tarefas devem ser finalziadas até o dia 16/10 para que assim se inicie a preparação final para a sprint.</t>
+  </si>
+  <si>
+    <t>FORMULARIO DO SITE</t>
+  </si>
+  <si>
+    <t>Foi feito uma reunião presencial para alinhamento do projeto, definição das métricas da dashboard e estruturação da apresentação, além do termino da calculadora, também ocorreu a redistribuição de algumas tarefas entre os integrantes.</t>
   </si>
 </sst>
 </file>
@@ -936,6 +939,57 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -961,424 +1015,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="127">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="130">
     <dxf>
       <font>
         <b val="0"/>
@@ -1549,7 +1192,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1630,6 +1273,396 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1685,7 +1718,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1829,7 +1862,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2066,7 +2099,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2315,7 +2348,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2411,7 +2444,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -2431,12 +2464,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2451,29 +2484,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2508,8 +2519,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2547,7 +2557,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -2567,12 +2577,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2587,7 +2597,29 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2622,7 +2654,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2700,7 +2733,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -3062,7 +3095,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -3155,188 +3188,188 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125" tableBorderDxfId="124">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128" tableBorderDxfId="127">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="123"/>
-    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="122"/>
-    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="121"/>
-    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="120"/>
+    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="126"/>
+    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="125"/>
+    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="124"/>
+    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="123"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADC66D5E-21F9-4392-BA43-F54A191A9B63}" name="Tabela2165712" displayName="Tabela2165712" ref="A20:C26" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADC66D5E-21F9-4392-BA43-F54A191A9B63}" name="Tabela2165712" displayName="Tabela2165712" ref="A20:C26" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" tableBorderDxfId="81">
   <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4032B737-C289-47F4-95E3-C10361BF2F0A}" name="NOME" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{819D06B1-F5CD-4FE5-A4A6-2CF334D95068}" name="PARTICIPAÇÃO" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{97FDEAA5-60F7-4DDE-8E46-7B446F1083F8}" name="JUSTIFICATIVA" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{4032B737-C289-47F4-95E3-C10361BF2F0A}" name="NOME" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{819D06B1-F5CD-4FE5-A4A6-2CF334D95068}" name="PARTICIPAÇÃO" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{97FDEAA5-60F7-4DDE-8E46-7B446F1083F8}" name="JUSTIFICATIVA" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D12" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D12" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76" tableBorderDxfId="75">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D12">
     <sortCondition ref="B5:B12"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A21:C27" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66" tableBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A21:C27" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" tableBorderDxfId="68">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D13" totalsRowShown="0" headerRowDxfId="61" tableBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D13" totalsRowShown="0" headerRowDxfId="64" tableBorderDxfId="63">
   <autoFilter ref="A7:D13" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I15" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" tableBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I15" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
   <autoFilter ref="F7:I15" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F8:I10">
     <sortCondition ref="H7:H10"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118" tableBorderDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121" tableBorderDxfId="120">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="116"/>
-    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="115"/>
-    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="119"/>
+    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="118"/>
+    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="117"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A21:C26" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112" tableBorderDxfId="111">
-  <autoFilter ref="A21:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="110"/>
-    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="109"/>
-    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="108"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27B233F8-A460-42F9-9C4B-D98237F9F3D3}" name="Tabela14" displayName="Tabela14" ref="A4:D12" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C2D86245-7317-4053-ADDF-3F8FD7BEFC06}" name="O QUE FAZER" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{C26B0139-2C07-4349-AB58-411D0BA2D235}" name="PRAZOS DE ENTREGA" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{54052D0A-0E1C-4DCA-874B-4E2C01A00642}" name="RESPONSAVEL" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{1D01342F-890F-4F70-B68D-C2CBD506803F}" name="SITUAÇÃO" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D12" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" tableBorderDxfId="105">
-  <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="104"/>
-    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="103"/>
-    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="102"/>
-    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="101"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{5674DB64-0624-4B89-832A-98DC1DCAC731}" name="Tabela213" displayName="Tabela213" ref="A21:C27" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{BF86BF98-CE38-41FB-8452-1B2D9F3A5CDD}" name="NOME" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{A1EE796B-230F-49D2-9449-2AB095E6AA66}" name="PARTICIPAÇÃO" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{1A87248E-2071-4015-A55F-FC85F19BB5DA}" name="JUSTIFICATIVA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{324E0C07-8EA6-4B35-87D9-DE2AED0640C1}" name="Tabela2168" displayName="Tabela2168" ref="A21:C26" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99" tableBorderDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{324E0C07-8EA6-4B35-87D9-DE2AED0640C1}" name="Tabela2168" displayName="Tabela2168" ref="A21:C26" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115" tableBorderDxfId="114">
   <autoFilter ref="A21:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{7E69ED47-85F2-43DC-B8CC-4924F8C0FE05}" name="NOME" dataDxfId="97"/>
-    <tableColumn id="2" xr3:uid="{B1BCA94B-0C82-47D2-B9B6-BC7C8CA91DCD}" name="PARTICIPAÇÃO" dataDxfId="96"/>
-    <tableColumn id="3" xr3:uid="{390953B5-3673-4E41-9F50-7739FFB48EB0}" name="JUSTIFICATIVA" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{7E69ED47-85F2-43DC-B8CC-4924F8C0FE05}" name="NOME" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{B1BCA94B-0C82-47D2-B9B6-BC7C8CA91DCD}" name="PARTICIPAÇÃO" dataDxfId="112"/>
+    <tableColumn id="3" xr3:uid="{390953B5-3673-4E41-9F50-7739FFB48EB0}" name="JUSTIFICATIVA" dataDxfId="111"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{622E7481-4404-4510-A294-DB4533FAC9CB}" name="Tabela1159" displayName="Tabela1159" ref="A4:D12" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93" tableBorderDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{622E7481-4404-4510-A294-DB4533FAC9CB}" name="Tabela1159" displayName="Tabela1159" ref="A4:D12" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109" tableBorderDxfId="108">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{33BD1B29-8219-42DE-AF54-F8304F91F6A5}" name="O QUE FAZER" dataDxfId="91"/>
-    <tableColumn id="2" xr3:uid="{0E591C9C-0DA1-4DA3-9361-03AE94548CB9}" name="PRAZOS DE ENTREGA" dataDxfId="90"/>
-    <tableColumn id="3" xr3:uid="{0FB61BFF-2541-43B4-A641-1D585232AA7A}" name="RESPONSAVEL" dataDxfId="89"/>
-    <tableColumn id="4" xr3:uid="{8F7A2B55-04BC-4428-88AC-1B5C144A9201}" name="SITUAÇÃO" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{33BD1B29-8219-42DE-AF54-F8304F91F6A5}" name="O QUE FAZER" dataDxfId="107"/>
+    <tableColumn id="2" xr3:uid="{0E591C9C-0DA1-4DA3-9361-03AE94548CB9}" name="PRAZOS DE ENTREGA" dataDxfId="106"/>
+    <tableColumn id="3" xr3:uid="{0FB61BFF-2541-43B4-A641-1D585232AA7A}" name="RESPONSAVEL" dataDxfId="105"/>
+    <tableColumn id="4" xr3:uid="{8F7A2B55-04BC-4428-88AC-1B5C144A9201}" name="SITUAÇÃO" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D12" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86" tableBorderDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D12" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102" tableBorderDxfId="101">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D12">
     <sortCondition ref="B5:B12"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="81"/>
+    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="99"/>
+    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="98"/>
+    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A21:C27" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79" tableBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A21:C27" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95" tableBorderDxfId="94">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{15EA983F-EF1E-40AD-8836-3919E5A2903E}" name="Tabela115465" displayName="Tabela115465" ref="A4:D11" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47" tableBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{15EA983F-EF1E-40AD-8836-3919E5A2903E}" name="Tabela115465" displayName="Tabela115465" ref="A4:D11" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89" tableBorderDxfId="88">
   <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D11">
     <sortCondition ref="B5:B11"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{179C583B-654D-4EA9-A6B1-98DC1306F4F6}" name="O QUE FAZER" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{BD210812-ED62-4497-BF8A-29BECC6FE272}" name="PRAZOS DE ENTREGA" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{316BEE82-6E8F-44CD-8CE2-3E31EFC8278A}" name="RESPONSAVEL" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{AEB6E40F-2D8E-4E23-8D61-0119E828DFD9}" name="SITUAÇÃO" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{179C583B-654D-4EA9-A6B1-98DC1306F4F6}" name="O QUE FAZER" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{BD210812-ED62-4497-BF8A-29BECC6FE272}" name="PRAZOS DE ENTREGA" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{316BEE82-6E8F-44CD-8CE2-3E31EFC8278A}" name="RESPONSAVEL" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{AEB6E40F-2D8E-4E23-8D61-0119E828DFD9}" name="SITUAÇÃO" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3665,12 +3698,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3681,7 +3714,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3692,7 +3725,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -3707,26 +3740,26 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="1"/>
-    <col min="7" max="7" width="7.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="7.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -3734,8 +3767,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -3747,7 +3780,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -3765,7 +3798,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>45</v>
       </c>
@@ -3783,7 +3816,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
@@ -3797,7 +3830,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>33</v>
       </c>
@@ -3817,7 +3850,7 @@
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
     </row>
-    <row r="8" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>46</v>
       </c>
@@ -3837,7 +3870,7 @@
       <c r="K8" s="22"/>
       <c r="L8" s="21"/>
     </row>
-    <row r="9" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -3857,7 +3890,7 @@
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
     </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
@@ -3877,7 +3910,7 @@
       <c r="K10" s="22"/>
       <c r="L10" s="21"/>
     </row>
-    <row r="11" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>48</v>
       </c>
@@ -3897,7 +3930,7 @@
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
@@ -3917,7 +3950,7 @@
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
@@ -3925,7 +3958,7 @@
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="1:12" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
@@ -3939,7 +3972,7 @@
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:12" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
         <v>58</v>
       </c>
@@ -3947,26 +3980,26 @@
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
     </row>
-    <row r="16" spans="1:12" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="34"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="37"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="39"/>
     </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
@@ -3976,7 +4009,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -3990,7 +4023,7 @@
         <v>45575</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4002,7 +4035,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -4014,7 +4047,7 @@
         <v>0.69444444444444442</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -4028,7 +4061,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -4040,7 +4073,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -4052,7 +4085,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -4079,32 +4112,32 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="10" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="11" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="4" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="5" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="6" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:K12">
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="7" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="8" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="9" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4141,24 +4174,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA47C666-6B9B-4ED9-8062-81E393DBE6A0}">
-  <dimension ref="A1:I27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F2CA3B-B5A6-43F9-B50E-5B07F700AEBF}">
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:D18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="40.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="7.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -4166,8 +4205,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -4179,7 +4218,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4197,7 +4236,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>45</v>
       </c>
@@ -4208,28 +4247,28 @@
         <v>12</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="6">
-        <v>45581</v>
+      <c r="B6" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>33</v>
       </c>
@@ -4240,24 +4279,36 @@
         <v>11</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+    </row>
+    <row r="8" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="B8" s="6">
         <v>45581</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="21"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="21"/>
+    </row>
+    <row r="9" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -4265,13 +4316,19 @@
         <v>45581</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+    </row>
+    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
@@ -4279,15 +4336,21 @@
         <v>45581</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="21"/>
+    </row>
+    <row r="11" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B11" s="6">
         <v>45581</v>
@@ -4298,58 +4361,83 @@
       <c r="D11" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="B12" s="6">
+        <v>45581</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+    </row>
+    <row r="13" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+    </row>
+    <row r="14" spans="1:12" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
       <c r="D14" s="27"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+    </row>
+    <row r="15" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
     </row>
-    <row r="16" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="34"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="37"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="39"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
@@ -4359,7 +4447,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -4370,10 +4458,10 @@
         <v>7</v>
       </c>
       <c r="D21" s="4">
-        <v>45576</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4385,7 +4473,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -4394,36 +4482,38 @@
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="7">
-        <v>0.68055555555555558</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.4861111111111111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="D24" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="8">
-        <v>0.69166666666666665</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.49861111111111112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>14</v>
@@ -4433,10 +4523,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="5"/>
       <c r="D27" s="3">
         <f>IF(D25="","",D25-D23)</f>
-        <v>1.1111111111111072E-2</v>
+        <v>1.2500000000000011E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4448,28 +4545,39 @@
     <mergeCell ref="A15:D18"/>
     <mergeCell ref="A20:C20"/>
   </mergeCells>
-  <conditionalFormatting sqref="B22:B26">
-    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
+  <conditionalFormatting sqref="B22:B27">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+      <formula>"Pendente"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8:K12">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+      <formula>"Finalizada"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+      <formula>"Em Andamento"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A26" xr:uid="{59CFC1D0-2CAA-43D4-A762-223F4FFFA1B2}">
-      <formula1>"João Pedro Ferraz, Lucas Aiello, Miguel Angel, Shelly Nadudvari, Thiago Sanchez,"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8:J12 C5:C12" xr:uid="{A1A97AEF-F65A-41A9-8263-EA54CE32129D}">
+      <formula1>$A$22:$A$27</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4480,24 +4588,18 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2B357CC2-7824-413D-9549-3CFC67866BDF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D583391-A12D-41E1-9CAE-047B54D55EAC}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D12</xm:sqref>
+          <xm:sqref>K8:K12 D5:D12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{71C13E2F-B2BD-410D-82BC-0528D1463BA6}">
-          <x14:formula1>
-            <xm:f>Quinta!$A$22:$A$27</xm:f>
-          </x14:formula1>
-          <xm:sqref>C5:C12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8D35B9F6-D63E-435F-9312-45B566A93C5E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FD2756DD-5DED-4AD9-A4C8-983EDEC7E836}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B22:B26</xm:sqref>
+          <xm:sqref>B22:B27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4513,17 +4615,17 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -4531,8 +4633,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -4544,7 +4646,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4562,7 +4664,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>45</v>
       </c>
@@ -4580,7 +4682,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
@@ -4594,7 +4696,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>33</v>
       </c>
@@ -4608,7 +4710,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>46</v>
       </c>
@@ -4622,7 +4724,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -4636,7 +4738,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
@@ -4650,7 +4752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>51</v>
       </c>
@@ -4664,7 +4766,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>61</v>
       </c>
@@ -4678,8 +4780,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
@@ -4687,34 +4789,34 @@
       <c r="C14" s="26"/>
       <c r="D14" s="27"/>
     </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
     </row>
-    <row r="16" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="34"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="37"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="39"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
@@ -4724,7 +4826,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -4738,7 +4840,7 @@
         <v>45577</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4750,7 +4852,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -4762,7 +4864,7 @@
         <v>0.63888888888888884</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -4774,7 +4876,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -4786,7 +4888,7 @@
         <v>0.64375000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -4798,7 +4900,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D27" s="3">
         <f>IF(D25="","",D25-D23)</f>
         <v>4.8611111111112049E-3</v>
@@ -4814,21 +4916,21 @@
     <mergeCell ref="A20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B26">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4878,17 +4980,17 @@
       <selection activeCell="D27" sqref="A1:D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -4896,8 +4998,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -4909,7 +5011,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4927,7 +5029,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>45</v>
       </c>
@@ -4945,7 +5047,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
@@ -4959,7 +5061,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>33</v>
       </c>
@@ -4973,7 +5075,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>46</v>
       </c>
@@ -4987,7 +5089,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -5001,7 +5103,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
@@ -5015,7 +5117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>51</v>
       </c>
@@ -5029,7 +5131,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>61</v>
       </c>
@@ -5043,8 +5145,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
@@ -5052,34 +5154,34 @@
       <c r="C14" s="26"/>
       <c r="D14" s="27"/>
     </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
     </row>
-    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="34"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="37"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="39"/>
     </row>
-    <row r="19" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
@@ -5089,7 +5191,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -5103,7 +5205,7 @@
         <v>45579</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -5115,7 +5217,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -5127,7 +5229,7 @@
         <v>0.59236111111111112</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -5139,7 +5241,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -5151,7 +5253,7 @@
         <v>0.60972222222222228</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -5163,7 +5265,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -5186,21 +5288,21 @@
     <mergeCell ref="A20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5241,21 +5343,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236B7F47-06D8-4355-B975-BA6E381EB758}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -5263,8 +5365,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -5276,7 +5378,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5294,7 +5396,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>45</v>
       </c>
@@ -5312,7 +5414,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
@@ -5326,7 +5428,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>46</v>
       </c>
@@ -5340,7 +5442,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>47</v>
       </c>
@@ -5354,7 +5456,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>54</v>
       </c>
@@ -5368,7 +5470,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>51</v>
       </c>
@@ -5382,7 +5484,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>61</v>
       </c>
@@ -5396,8 +5498,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>29</v>
       </c>
@@ -5405,34 +5507,34 @@
       <c r="C13" s="26"/>
       <c r="D13" s="27"/>
     </row>
-    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
       <c r="D14" s="33"/>
     </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="34"/>
       <c r="B15" s="35"/>
       <c r="C15" s="35"/>
       <c r="D15" s="36"/>
     </row>
-    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="37"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
       <c r="D17" s="39"/>
     </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
         <v>19</v>
       </c>
@@ -5442,7 +5544,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
@@ -5456,7 +5558,7 @@
         <v>45580</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -5468,7 +5570,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -5480,7 +5582,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -5492,7 +5594,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -5504,7 +5606,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -5516,7 +5618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -5539,21 +5641,21 @@
     <mergeCell ref="A19:C19"/>
   </mergeCells>
   <conditionalFormatting sqref="B21:B26">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D11">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5598,17 +5700,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -5616,8 +5718,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -5629,7 +5731,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5647,7 +5749,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>34</v>
       </c>
@@ -5665,7 +5767,7 @@
       <c r="H5" s="20"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>44</v>
       </c>
@@ -5679,7 +5781,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>35</v>
       </c>
@@ -5693,7 +5795,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>50</v>
       </c>
@@ -5707,7 +5809,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -5721,7 +5823,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -5735,7 +5837,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -5749,7 +5851,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>51</v>
       </c>
@@ -5763,8 +5865,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
@@ -5772,7 +5874,7 @@
       <c r="C14" s="26"/>
       <c r="D14" s="27"/>
     </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
         <v>52</v>
       </c>
@@ -5780,26 +5882,26 @@
       <c r="C15" s="40"/>
       <c r="D15" s="41"/>
     </row>
-    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="42"/>
       <c r="B16" s="43"/>
       <c r="C16" s="43"/>
       <c r="D16" s="44"/>
     </row>
-    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="42"/>
       <c r="B17" s="43"/>
       <c r="C17" s="43"/>
       <c r="D17" s="44"/>
     </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="45"/>
       <c r="B18" s="46"/>
       <c r="C18" s="46"/>
       <c r="D18" s="47"/>
     </row>
-    <row r="19" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
@@ -5809,7 +5911,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -5823,7 +5925,7 @@
         <v>45574</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -5835,7 +5937,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -5847,7 +5949,7 @@
         <v>0.68194444444444446</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -5861,7 +5963,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -5873,7 +5975,7 @@
         <v>0.7055555555555556</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -5885,7 +5987,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -5908,21 +6010,21 @@
     <mergeCell ref="A20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5975,21 +6077,21 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="37" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="31.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>36</v>
       </c>
@@ -6002,8 +6104,8 @@
       <c r="H1" s="26"/>
       <c r="I1" s="27"/>
     </row>
-    <row r="2" spans="1:9" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>49</v>
       </c>
@@ -6017,44 +6119,44 @@
       <c r="H3" s="26"/>
       <c r="I3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="60"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51"/>
       <c r="F4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="59"/>
-      <c r="I4" s="60"/>
-    </row>
-    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+    </row>
+    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="62"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
       <c r="F5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="61" t="s">
+      <c r="G5" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="62"/>
-    </row>
-    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>3</v>
       </c>
@@ -6080,7 +6182,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>45</v>
       </c>
@@ -6106,7 +6208,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>27</v>
       </c>
@@ -6132,7 +6234,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>33</v>
       </c>
@@ -6158,7 +6260,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>46</v>
       </c>
@@ -6184,7 +6286,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>47</v>
       </c>
@@ -6210,7 +6312,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>54</v>
       </c>
@@ -6236,7 +6338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
@@ -6254,7 +6356,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
@@ -6272,7 +6374,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
         <v>30</v>
       </c>
@@ -6284,7 +6386,7 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="31" t="s">
         <v>60</v>
       </c>
@@ -6292,115 +6394,123 @@
       <c r="C17" s="32"/>
       <c r="D17" s="33"/>
     </row>
-    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="34"/>
       <c r="B18" s="35"/>
       <c r="C18" s="35"/>
       <c r="D18" s="36"/>
     </row>
-    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="34"/>
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
       <c r="D19" s="36"/>
     </row>
-    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="37"/>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
       <c r="D20" s="39"/>
     </row>
-    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21" s="13"/>
     </row>
-    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="63" t="s">
+    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="65"/>
-    </row>
-    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="70" t="s">
+      <c r="B22" s="55"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="56"/>
+    </row>
+    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="71"/>
-      <c r="C23" s="66" t="s">
+      <c r="B23" s="62"/>
+      <c r="C23" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="67"/>
-    </row>
-    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="72" t="s">
+      <c r="D23" s="58"/>
+    </row>
+    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="68"/>
-      <c r="C24" s="68" t="s">
+      <c r="B24" s="59"/>
+      <c r="C24" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="69"/>
-    </row>
-    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="73" t="s">
+      <c r="D24" s="60"/>
+    </row>
+    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57" t="s">
+      <c r="B25" s="48"/>
+      <c r="C25" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="58"/>
-    </row>
-    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="48" t="s">
+      <c r="D25" s="49"/>
+    </row>
+    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49" t="s">
+      <c r="B26" s="66"/>
+      <c r="C26" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="55"/>
-    </row>
-    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="50" t="s">
+      <c r="D26" s="72"/>
+    </row>
+    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51" t="s">
+      <c r="B27" s="68"/>
+      <c r="C27" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="56"/>
-    </row>
-    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
+      <c r="D27" s="73"/>
+    </row>
+    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49" t="s">
+      <c r="B28" s="66"/>
+      <c r="C28" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="55"/>
-    </row>
-    <row r="29" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="52" t="s">
+      <c r="D28" s="72"/>
+    </row>
+    <row r="29" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53" t="s">
+      <c r="B29" s="70"/>
+      <c r="C29" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="54"/>
-    </row>
-    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D29" s="71"/>
+    </row>
+    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D20"/>
@@ -6417,24 +6527,16 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="D8:D15 I8:I15">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ata sábado e ícon Quem Samos
</commit_message>
<xml_diff>
--- a/Documentação/ATAs_de_Reuniao/Sprint 2/Semana 1010/Grupo4_ATA_Semana1010.xlsx
+++ b/Documentação/ATAs_de_Reuniao/Sprint 2/Semana 1010/Grupo4_ATA_Semana1010.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpfer\OneDrive\Documentos\SPTECH\PI\SPRINT\Sprint-SPTECH\Documentação\ATAs_de_Reuniao\Sprint 2\Semana 1010\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4fd29038e46714d/Área de Trabalho/SPTECH/Pesquisa e Inovação/Sprint-SPTECH/Documentação/ATAs_de_Reuniao/Sprint 2/Semana 1010/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3E68C8-49F1-4090-BEAF-5EAAC91AB15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{DB3E68C8-49F1-4090-BEAF-5EAAC91AB15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85918BF5-C5DE-4BB1-80E3-42420D18D647}"/>
   <bookViews>
-    <workbookView xWindow="4824" yWindow="3360" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="2" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" firstSheet="1" activeTab="7" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DE DADOS" sheetId="2" state="hidden" r:id="rId1"/>
     <sheet name="Quinta" sheetId="1" r:id="rId2"/>
     <sheet name="Sexta" sheetId="19" r:id="rId3"/>
-    <sheet name="Sábado" sheetId="17" r:id="rId4"/>
+    <sheet name="Sábado" sheetId="20" r:id="rId4"/>
     <sheet name="Segunda" sheetId="13" r:id="rId5"/>
     <sheet name="Terça" sheetId="18" r:id="rId6"/>
     <sheet name="Quarta" sheetId="15" r:id="rId7"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="68">
   <si>
     <t>NOME</t>
   </si>
@@ -234,9 +234,6 @@
     <t>16/10/2024</t>
   </si>
   <si>
-    <t>Conferimos novamente o que estava pendente no trabalho. Cada membro comunicou o que seria feito durante o fim de semana para apresentarmos na próxima daily, na segunda-feira.</t>
-  </si>
-  <si>
     <t>Falamos a respeito da Dashboard e as KPI's que terão, os slides e o digrama de solução</t>
   </si>
   <si>
@@ -247,6 +244,9 @@
   </si>
   <si>
     <t>Foi feito uma reunião presencial para alinhamento do projeto, definição das métricas da dashboard e estruturação da apresentação, além do termino da calculadora, também ocorreu a redistribuição de algumas tarefas entre os integrantes.</t>
+  </si>
+  <si>
+    <t>As últimas pendencias do projeto foram conversadas e distribuídas entre os membros. Decidimos os próximos passos do projeto. Estudamos os formulários de outras empresas já estabelecidas no mercado para comparação com o formulário do nosso projeto. Decidimos as cores e os últimos ajustes das métricas e de nossa dashboard.</t>
   </si>
 </sst>
 </file>
@@ -939,6 +939,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -988,40 +1015,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="130">
+  <dxfs count="133">
     <dxf>
       <font>
         <b val="0"/>
@@ -1563,6 +1563,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2693,7 +2723,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -2713,12 +2743,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2733,29 +2763,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2790,8 +2798,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2829,7 +2836,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -2849,12 +2856,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2869,7 +2876,29 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2904,7 +2933,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3188,188 +3218,188 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128" tableBorderDxfId="127">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="132" dataDxfId="131" tableBorderDxfId="130">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="126"/>
-    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="125"/>
-    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="124"/>
-    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="123"/>
+    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="129"/>
+    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="128"/>
+    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="127"/>
+    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADC66D5E-21F9-4392-BA43-F54A191A9B63}" name="Tabela2165712" displayName="Tabela2165712" ref="A20:C26" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" tableBorderDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADC66D5E-21F9-4392-BA43-F54A191A9B63}" name="Tabela2165712" displayName="Tabela2165712" ref="A20:C26" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85" tableBorderDxfId="84">
   <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4032B737-C289-47F4-95E3-C10361BF2F0A}" name="NOME" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{819D06B1-F5CD-4FE5-A4A6-2CF334D95068}" name="PARTICIPAÇÃO" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{97FDEAA5-60F7-4DDE-8E46-7B446F1083F8}" name="JUSTIFICATIVA" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{4032B737-C289-47F4-95E3-C10361BF2F0A}" name="NOME" dataDxfId="83"/>
+    <tableColumn id="2" xr3:uid="{819D06B1-F5CD-4FE5-A4A6-2CF334D95068}" name="PARTICIPAÇÃO" dataDxfId="82"/>
+    <tableColumn id="3" xr3:uid="{97FDEAA5-60F7-4DDE-8E46-7B446F1083F8}" name="JUSTIFICATIVA" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D12" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76" tableBorderDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D12" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79" tableBorderDxfId="78">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D12">
     <sortCondition ref="B5:B12"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="72"/>
-    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A21:C27" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" tableBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A21:C27" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72" tableBorderDxfId="71">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D13" totalsRowShown="0" headerRowDxfId="64" tableBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D13" totalsRowShown="0" headerRowDxfId="67" tableBorderDxfId="66">
   <autoFilter ref="A7:D13" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="63"/>
+    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I15" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I15" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60" tableBorderDxfId="59">
   <autoFilter ref="F7:I15" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F8:I10">
     <sortCondition ref="H7:H10"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121" tableBorderDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124" tableBorderDxfId="123">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="119"/>
-    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="118"/>
-    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="117"/>
+    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="122"/>
+    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="121"/>
+    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="120"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27B233F8-A460-42F9-9C4B-D98237F9F3D3}" name="Tabela14" displayName="Tabela14" ref="A4:D12" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27B233F8-A460-42F9-9C4B-D98237F9F3D3}" name="Tabela14" displayName="Tabela14" ref="A4:D12" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118" tableBorderDxfId="117">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C2D86245-7317-4053-ADDF-3F8FD7BEFC06}" name="O QUE FAZER" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{C26B0139-2C07-4349-AB58-411D0BA2D235}" name="PRAZOS DE ENTREGA" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{54052D0A-0E1C-4DCA-874B-4E2C01A00642}" name="RESPONSAVEL" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{1D01342F-890F-4F70-B68D-C2CBD506803F}" name="SITUAÇÃO" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{C2D86245-7317-4053-ADDF-3F8FD7BEFC06}" name="O QUE FAZER" dataDxfId="116"/>
+    <tableColumn id="2" xr3:uid="{C26B0139-2C07-4349-AB58-411D0BA2D235}" name="PRAZOS DE ENTREGA" dataDxfId="115"/>
+    <tableColumn id="3" xr3:uid="{54052D0A-0E1C-4DCA-874B-4E2C01A00642}" name="RESPONSAVEL" dataDxfId="114"/>
+    <tableColumn id="4" xr3:uid="{1D01342F-890F-4F70-B68D-C2CBD506803F}" name="SITUAÇÃO" dataDxfId="113"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{5674DB64-0624-4B89-832A-98DC1DCAC731}" name="Tabela213" displayName="Tabela213" ref="A21:C27" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{5674DB64-0624-4B89-832A-98DC1DCAC731}" name="Tabela213" displayName="Tabela213" ref="A21:C27" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111" tableBorderDxfId="110">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BF86BF98-CE38-41FB-8452-1B2D9F3A5CDD}" name="NOME" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{A1EE796B-230F-49D2-9449-2AB095E6AA66}" name="PARTICIPAÇÃO" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{1A87248E-2071-4015-A55F-FC85F19BB5DA}" name="JUSTIFICATIVA" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{BF86BF98-CE38-41FB-8452-1B2D9F3A5CDD}" name="NOME" dataDxfId="109"/>
+    <tableColumn id="2" xr3:uid="{A1EE796B-230F-49D2-9449-2AB095E6AA66}" name="PARTICIPAÇÃO" dataDxfId="108"/>
+    <tableColumn id="3" xr3:uid="{1A87248E-2071-4015-A55F-FC85F19BB5DA}" name="JUSTIFICATIVA" dataDxfId="107"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{324E0C07-8EA6-4B35-87D9-DE2AED0640C1}" name="Tabela2168" displayName="Tabela2168" ref="A21:C26" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115" tableBorderDxfId="114">
-  <autoFilter ref="A21:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{7E69ED47-85F2-43DC-B8CC-4924F8C0FE05}" name="NOME" dataDxfId="113"/>
-    <tableColumn id="2" xr3:uid="{B1BCA94B-0C82-47D2-B9B6-BC7C8CA91DCD}" name="PARTICIPAÇÃO" dataDxfId="112"/>
-    <tableColumn id="3" xr3:uid="{390953B5-3673-4E41-9F50-7739FFB48EB0}" name="JUSTIFICATIVA" dataDxfId="111"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{A02AEA0D-D230-4941-AB5A-C3A924D0B4E2}" name="Tabela1415" displayName="Tabela1415" ref="A4:D12" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{6AF81835-78B3-48F1-8A28-C213FBAC6BD9}" name="O QUE FAZER" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{30A230F2-5BF0-470A-A0B8-10CBAE3652EC}" name="PRAZOS DE ENTREGA" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{10D1D69C-C683-4456-B5E3-2B5FBF84B7A1}" name="RESPONSAVEL" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{3EE42AAF-05EE-49CF-BBD2-DC0C19E432BF}" name="SITUAÇÃO" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{622E7481-4404-4510-A294-DB4533FAC9CB}" name="Tabela1159" displayName="Tabela1159" ref="A4:D12" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109" tableBorderDxfId="108">
-  <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{33BD1B29-8219-42DE-AF54-F8304F91F6A5}" name="O QUE FAZER" dataDxfId="107"/>
-    <tableColumn id="2" xr3:uid="{0E591C9C-0DA1-4DA3-9361-03AE94548CB9}" name="PRAZOS DE ENTREGA" dataDxfId="106"/>
-    <tableColumn id="3" xr3:uid="{0FB61BFF-2541-43B4-A641-1D585232AA7A}" name="RESPONSAVEL" dataDxfId="105"/>
-    <tableColumn id="4" xr3:uid="{8F7A2B55-04BC-4428-88AC-1B5C144A9201}" name="SITUAÇÃO" dataDxfId="104"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{6ADE6A5E-6FDC-44DC-80F8-1AD31F816010}" name="Tabela21316" displayName="Tabela21316" ref="A21:C27" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{DBD61C1A-2F48-409A-AFDF-4D5F7E59026B}" name="NOME" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{56698CBD-848E-4E76-8E3E-9FFC2B3D3827}" name="PARTICIPAÇÃO" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{0FB7F289-88CC-479A-A86D-8DB483B9A424}" name="JUSTIFICATIVA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D12" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102" tableBorderDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D12" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" tableBorderDxfId="104">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D12">
     <sortCondition ref="B5:B12"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="100"/>
-    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="99"/>
-    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="98"/>
-    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="97"/>
+    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="103"/>
+    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="102"/>
+    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="101"/>
+    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A21:C27" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95" tableBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A21:C27" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98" tableBorderDxfId="97">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="91"/>
+    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="95"/>
+    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{15EA983F-EF1E-40AD-8836-3919E5A2903E}" name="Tabela115465" displayName="Tabela115465" ref="A4:D11" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89" tableBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{15EA983F-EF1E-40AD-8836-3919E5A2903E}" name="Tabela115465" displayName="Tabela115465" ref="A4:D11" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92" tableBorderDxfId="91">
   <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D11">
     <sortCondition ref="B5:B11"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{179C583B-654D-4EA9-A6B1-98DC1306F4F6}" name="O QUE FAZER" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{BD210812-ED62-4497-BF8A-29BECC6FE272}" name="PRAZOS DE ENTREGA" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{316BEE82-6E8F-44CD-8CE2-3E31EFC8278A}" name="RESPONSAVEL" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{AEB6E40F-2D8E-4E23-8D61-0119E828DFD9}" name="SITUAÇÃO" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{179C583B-654D-4EA9-A6B1-98DC1306F4F6}" name="O QUE FAZER" dataDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{BD210812-ED62-4497-BF8A-29BECC6FE272}" name="PRAZOS DE ENTREGA" dataDxfId="89"/>
+    <tableColumn id="3" xr3:uid="{316BEE82-6E8F-44CD-8CE2-3E31EFC8278A}" name="RESPONSAVEL" dataDxfId="88"/>
+    <tableColumn id="4" xr3:uid="{AEB6E40F-2D8E-4E23-8D61-0119E828DFD9}" name="SITUAÇÃO" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3698,12 +3728,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3714,7 +3744,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3725,7 +3755,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -3743,23 +3773,23 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="7.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.90625" style="1"/>
+    <col min="7" max="7" width="7.90625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" style="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="12" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -3767,8 +3797,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -3780,7 +3810,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -3798,7 +3828,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>45</v>
       </c>
@@ -3816,7 +3846,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
@@ -3830,7 +3860,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
         <v>33</v>
       </c>
@@ -3850,7 +3880,7 @@
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
     </row>
-    <row r="8" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>46</v>
       </c>
@@ -3870,7 +3900,7 @@
       <c r="K8" s="22"/>
       <c r="L8" s="21"/>
     </row>
-    <row r="9" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -3890,7 +3920,7 @@
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
     </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
@@ -3910,7 +3940,7 @@
       <c r="K10" s="22"/>
       <c r="L10" s="21"/>
     </row>
-    <row r="11" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>48</v>
       </c>
@@ -3930,7 +3960,7 @@
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
@@ -3950,7 +3980,7 @@
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
@@ -3958,7 +3988,7 @@
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="1:12" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
@@ -3972,7 +4002,7 @@
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
         <v>58</v>
       </c>
@@ -3980,26 +4010,26 @@
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
     </row>
-    <row r="16" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="34"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="37"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="39"/>
     </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
@@ -4009,7 +4039,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -4023,7 +4053,7 @@
         <v>45575</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4035,7 +4065,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -4047,7 +4077,7 @@
         <v>0.69444444444444442</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -4061,7 +4091,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -4073,7 +4103,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -4085,7 +4115,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -4112,32 +4142,32 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="51" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="10" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="11" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="49" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="5" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:K12">
-    <cfRule type="cellIs" dxfId="46" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="7" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="8" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="9" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4177,27 +4207,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F2CA3B-B5A6-43F9-B50E-5B07F700AEBF}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="7.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.90625" style="1"/>
+    <col min="7" max="7" width="7.90625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" style="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="12" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -4205,8 +4235,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -4218,7 +4248,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4236,7 +4266,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>45</v>
       </c>
@@ -4254,7 +4284,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
@@ -4268,7 +4298,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
         <v>33</v>
       </c>
@@ -4288,9 +4318,9 @@
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
     </row>
-    <row r="8" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="6">
         <v>45581</v>
@@ -4308,7 +4338,7 @@
       <c r="K8" s="22"/>
       <c r="L8" s="21"/>
     </row>
-    <row r="9" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -4328,7 +4358,7 @@
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
     </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
@@ -4348,7 +4378,7 @@
       <c r="K10" s="22"/>
       <c r="L10" s="21"/>
     </row>
-    <row r="11" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>48</v>
       </c>
@@ -4368,7 +4398,7 @@
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
@@ -4388,7 +4418,7 @@
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
@@ -4396,7 +4426,7 @@
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="1:12" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
@@ -4410,34 +4440,34 @@
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
     </row>
-    <row r="16" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="34"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="37"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="39"/>
     </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
@@ -4447,7 +4477,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -4461,7 +4491,7 @@
         <v>45575</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4473,7 +4503,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -4485,7 +4515,7 @@
         <v>0.4861111111111111</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -4499,7 +4529,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -4511,7 +4541,7 @@
         <v>0.49861111111111112</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -4523,7 +4553,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -4534,6 +4564,440 @@
       <c r="D27" s="3">
         <f>IF(D25="","",D25-D23)</f>
         <v>1.2500000000000011E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D18"/>
+    <mergeCell ref="A20:C20"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B22:B27">
+    <cfRule type="cellIs" dxfId="46" priority="7" operator="equal">
+      <formula>"AUSENTE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="8" operator="equal">
+      <formula>"PRESENTE"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D12">
+    <cfRule type="cellIs" dxfId="44" priority="1" operator="equal">
+      <formula>"Finalizada"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
+      <formula>"Em Andamento"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
+      <formula>"Pendente"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8:K12">
+    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+      <formula>"Finalizada"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
+      <formula>"Em Andamento"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
+      <formula>"Pendente"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8:J12 C5:C12" xr:uid="{A1A97AEF-F65A-41A9-8263-EA54CE32129D}">
+      <formula1>$A$22:$A$27</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D583391-A12D-41E1-9CAE-047B54D55EAC}">
+          <x14:formula1>
+            <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>K8:K12 D5:D12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FD2756DD-5DED-4AD9-A4C8-983EDEC7E836}">
+          <x14:formula1>
+            <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>B22:B27</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8AB2E71-F167-4D03-8AA5-DF42D241EB70}">
+  <dimension ref="A1:L27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.90625" style="1"/>
+    <col min="7" max="7" width="7.90625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.90625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="6">
+        <v>45581</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+    </row>
+    <row r="6" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="6">
+        <v>45581</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+    </row>
+    <row r="8" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="6">
+        <v>45581</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="21"/>
+    </row>
+    <row r="9" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="6">
+        <v>45581</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+    </row>
+    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="6">
+        <v>45581</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="21"/>
+    </row>
+    <row r="11" spans="1:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="6">
+        <v>45581</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="6">
+        <v>45581</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+    </row>
+    <row r="13" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+    </row>
+    <row r="14" spans="1:12" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+    </row>
+    <row r="15" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
+    </row>
+    <row r="16" spans="1:12" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="34"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="36"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="34"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
+    </row>
+    <row r="18" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="39"/>
+    </row>
+    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4">
+        <v>45584</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="7">
+        <v>0.67013888888888884</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="8">
+        <v>0.68055555555555558</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="3">
+        <f>IF(D25="","",D25-D23)</f>
+        <v>1.0416666666666741E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4576,7 +5040,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8:J12 C5:C12" xr:uid="{A1A97AEF-F65A-41A9-8263-EA54CE32129D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8:J12 C5:C12" xr:uid="{E03EFD94-15C9-4268-9677-64241673106D}">
       <formula1>$A$22:$A$27</formula1>
     </dataValidation>
   </dataValidations>
@@ -4589,382 +5053,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D583391-A12D-41E1-9CAE-047B54D55EAC}">
-          <x14:formula1>
-            <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>K8:K12 D5:D12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FD2756DD-5DED-4AD9-A4C8-983EDEC7E836}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{48BE8245-5200-4F17-9615-6B00D0F67F36}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
           </x14:formula1>
           <xm:sqref>B22:B27</xm:sqref>
         </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3774AD0F-E7AD-4FE5-B16F-404B28A21F6A}">
-  <dimension ref="A1:I27"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="27"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-    </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="6">
-        <v>45581</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-    </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="6">
-        <v>45581</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="6">
-        <v>45581</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="6">
-        <v>45581</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="6">
-        <v>45581</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="6">
-        <v>45581</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="6">
-        <v>45581</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="33"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="36"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="36"/>
-    </row>
-    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="37"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="39"/>
-    </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="4">
-        <v>45577</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="7">
-        <v>0.63888888888888884</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="8">
-        <v>0.64375000000000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D27" s="3">
-        <f>IF(D25="","",D25-D23)</f>
-        <v>4.8611111111112049E-3</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="5">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:D18"/>
-    <mergeCell ref="A20:C20"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B22:B26">
-    <cfRule type="cellIs" dxfId="43" priority="4" operator="equal">
-      <formula>"AUSENTE"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
-      <formula>"PRESENTE"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
-      <formula>"Finalizada"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
-      <formula>"Em Andamento"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
-      <formula>"Pendente"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A26" xr:uid="{F68E03D4-F536-400E-AD8D-24616D2BDB2B}">
-      <formula1>"João Pedro Ferraz, Lucas Aiello, Miguel Angel, Shelly Nadudvari, Thiago Sanchez,"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-  </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C86E183D-236E-4451-8973-B75EC6E3BF4C}">
-          <x14:formula1>
-            <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>B22:B26</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{800333A3-8DD5-4B73-B295-47E99257F6E4}">
-          <x14:formula1>
-            <xm:f>Quinta!$A$22:$A$27</xm:f>
-          </x14:formula1>
-          <xm:sqref>C5:C12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1596508A-2F90-4B86-A8B8-BA63FF3B9DB7}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7DDBAB21-B0F7-4E35-9720-C1F328248523}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D12</xm:sqref>
+          <xm:sqref>K8:K12 D5:D12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4977,20 +5076,20 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D27" sqref="A1:D27"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -4998,8 +5097,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -5011,7 +5110,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5029,7 +5128,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>45</v>
       </c>
@@ -5047,7 +5146,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
@@ -5061,7 +5160,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
         <v>33</v>
       </c>
@@ -5075,7 +5174,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>46</v>
       </c>
@@ -5089,7 +5188,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -5103,7 +5202,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
@@ -5117,7 +5216,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>51</v>
       </c>
@@ -5131,7 +5230,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>61</v>
       </c>
@@ -5145,8 +5244,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
@@ -5154,34 +5253,34 @@
       <c r="C14" s="26"/>
       <c r="D14" s="27"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
     </row>
-    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="34"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="37"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="39"/>
     </row>
-    <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
@@ -5191,7 +5290,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -5205,7 +5304,7 @@
         <v>45579</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -5217,7 +5316,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -5229,7 +5328,7 @@
         <v>0.59236111111111112</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -5241,7 +5340,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -5253,7 +5352,7 @@
         <v>0.60972222222222228</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -5265,7 +5364,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -5347,17 +5446,17 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -5365,8 +5464,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -5378,7 +5477,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5396,7 +5495,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>45</v>
       </c>
@@ -5414,7 +5513,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
@@ -5428,7 +5527,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>46</v>
       </c>
@@ -5442,7 +5541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>47</v>
       </c>
@@ -5456,7 +5555,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>54</v>
       </c>
@@ -5470,7 +5569,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>51</v>
       </c>
@@ -5484,7 +5583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>61</v>
       </c>
@@ -5498,8 +5597,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="25" t="s">
         <v>29</v>
       </c>
@@ -5507,34 +5606,34 @@
       <c r="C13" s="26"/>
       <c r="D13" s="27"/>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
       <c r="D14" s="33"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="34"/>
       <c r="B15" s="35"/>
       <c r="C15" s="35"/>
       <c r="D15" s="36"/>
     </row>
-    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="37"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
       <c r="D17" s="39"/>
     </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="28" t="s">
         <v>19</v>
       </c>
@@ -5544,7 +5643,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
@@ -5558,7 +5657,7 @@
         <v>45580</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -5570,7 +5669,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -5582,7 +5681,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -5594,7 +5693,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -5606,7 +5705,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -5618,7 +5717,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -5700,17 +5799,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
@@ -5718,8 +5817,8 @@
       <c r="C1" s="26"/>
       <c r="D1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
@@ -5731,7 +5830,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5749,7 +5848,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>34</v>
       </c>
@@ -5767,7 +5866,7 @@
       <c r="H5" s="20"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>44</v>
       </c>
@@ -5781,7 +5880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>35</v>
       </c>
@@ -5795,7 +5894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>50</v>
       </c>
@@ -5809,7 +5908,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -5823,7 +5922,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -5837,7 +5936,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -5851,7 +5950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>51</v>
       </c>
@@ -5865,8 +5964,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
@@ -5874,7 +5973,7 @@
       <c r="C14" s="26"/>
       <c r="D14" s="27"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
         <v>52</v>
       </c>
@@ -5882,26 +5981,26 @@
       <c r="C15" s="40"/>
       <c r="D15" s="41"/>
     </row>
-    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="42"/>
       <c r="B16" s="43"/>
       <c r="C16" s="43"/>
       <c r="D16" s="44"/>
     </row>
-    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="42"/>
       <c r="B17" s="43"/>
       <c r="C17" s="43"/>
       <c r="D17" s="44"/>
     </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="45"/>
       <c r="B18" s="46"/>
       <c r="C18" s="46"/>
       <c r="D18" s="47"/>
     </row>
-    <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="28" t="s">
         <v>19</v>
       </c>
@@ -5911,7 +6010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -5925,7 +6024,7 @@
         <v>45574</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -5937,7 +6036,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -5949,7 +6048,7 @@
         <v>0.68194444444444446</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -5963,7 +6062,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -5975,7 +6074,7 @@
         <v>0.7055555555555556</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -5987,7 +6086,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -6073,25 +6172,25 @@
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.453125" style="1" customWidth="1"/>
     <col min="6" max="6" width="37" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="31.08984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="25" t="s">
         <v>36</v>
       </c>
@@ -6104,8 +6203,8 @@
       <c r="H1" s="26"/>
       <c r="I1" s="27"/>
     </row>
-    <row r="2" spans="1:9" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>49</v>
       </c>
@@ -6119,44 +6218,44 @@
       <c r="H3" s="26"/>
       <c r="I3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="51"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="60"/>
       <c r="F4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="51"/>
-    </row>
-    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H4" s="59"/>
+      <c r="I4" s="60"/>
+    </row>
+    <row r="5" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="62"/>
       <c r="F5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
-    </row>
-    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="61"/>
+      <c r="I5" s="62"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>3</v>
       </c>
@@ -6182,7 +6281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
         <v>45</v>
       </c>
@@ -6208,7 +6307,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
         <v>27</v>
       </c>
@@ -6234,7 +6333,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
         <v>33</v>
       </c>
@@ -6260,7 +6359,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>46</v>
       </c>
@@ -6286,7 +6385,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>47</v>
       </c>
@@ -6312,7 +6411,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>54</v>
       </c>
@@ -6338,7 +6437,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
@@ -6356,7 +6455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
@@ -6374,7 +6473,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="25" t="s">
         <v>30</v>
       </c>
@@ -6386,7 +6485,7 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="31" t="s">
         <v>60</v>
       </c>
@@ -6394,123 +6493,115 @@
       <c r="C17" s="32"/>
       <c r="D17" s="33"/>
     </row>
-    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="34"/>
       <c r="B18" s="35"/>
       <c r="C18" s="35"/>
       <c r="D18" s="36"/>
     </row>
-    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="34"/>
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
       <c r="D19" s="36"/>
     </row>
-    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="37"/>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
       <c r="D20" s="39"/>
     </row>
-    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21" s="13"/>
     </row>
-    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="54" t="s">
+    <row r="22" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="56"/>
-    </row>
-    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="61" t="s">
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="65"/>
+    </row>
+    <row r="23" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="62"/>
-      <c r="C23" s="57" t="s">
+      <c r="B23" s="71"/>
+      <c r="C23" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="58"/>
-    </row>
-    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="63" t="s">
+      <c r="D23" s="67"/>
+    </row>
+    <row r="24" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59" t="s">
+      <c r="B24" s="68"/>
+      <c r="C24" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="60"/>
-    </row>
-    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="64" t="s">
+      <c r="D24" s="69"/>
+    </row>
+    <row r="25" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48" t="s">
+      <c r="B25" s="57"/>
+      <c r="C25" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="49"/>
-    </row>
-    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="65" t="s">
+      <c r="D25" s="58"/>
+    </row>
+    <row r="26" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="66"/>
-      <c r="C26" s="66" t="s">
+      <c r="B26" s="49"/>
+      <c r="C26" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="72"/>
-    </row>
-    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="67" t="s">
+      <c r="D26" s="55"/>
+    </row>
+    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68" t="s">
+      <c r="B27" s="51"/>
+      <c r="C27" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="73"/>
-    </row>
-    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="65" t="s">
+      <c r="D27" s="56"/>
+    </row>
+    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66" t="s">
+      <c r="B28" s="49"/>
+      <c r="C28" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="72"/>
-    </row>
-    <row r="29" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="69" t="s">
+      <c r="D28" s="55"/>
+    </row>
+    <row r="29" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="70"/>
-      <c r="C29" s="70" t="s">
+      <c r="B29" s="53"/>
+      <c r="C29" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="71"/>
-    </row>
-    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="D29" s="54"/>
+    </row>
+    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A28:B28"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D20"/>
@@ -6527,6 +6618,14 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="D8:D15 I8:I15">

</xml_diff>